<commit_message>
Update defect tracker template
</commit_message>
<xml_diff>
--- a/Defect_Tracker Template_v0.1.xlsx
+++ b/Defect_Tracker Template_v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chhaj\OneDrive\Desktop\gaurav\college\Infosys project\Internship_artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03042BB0-9012-48A7-8AA3-AD7A8FBC54E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7FCE98-86FA-4BED-965C-926A5C9B9464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Sprint 4</t>
   </si>
   <si>
-    <t>Arjun</t>
-  </si>
-  <si>
     <t>Functional</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Team B</t>
+  </si>
+  <si>
+    <t>Aryan</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="9">
         <v>45963</v>
@@ -694,22 +694,22 @@
         <v>17</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="I2" s="9">
         <v>45964</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.3">
@@ -717,34 +717,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9">
         <v>45964</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="I3" s="9">
         <v>45965</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.3">
@@ -752,34 +752,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9">
         <v>45965</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="I4" s="9">
         <v>45966</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.3">
@@ -787,34 +787,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9">
         <v>45967</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="I5" s="9">
         <v>45968</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.3">
@@ -822,34 +822,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="9">
         <v>45968</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="9">
         <v>45969</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -857,34 +857,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="9">
         <v>45970</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="I7" s="9">
         <v>45970</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="24" x14ac:dyDescent="0.3">
@@ -892,34 +892,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="9">
         <v>45971</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="I8" s="9">
         <v>45972</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="36" x14ac:dyDescent="0.3">
@@ -927,34 +927,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="9">
         <v>45972</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="I9" s="9">
         <v>45973</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -1149,6 +1149,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F50FC49184C87E449886FB52439922C9" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85b7e58c3d8889ba0673e7b34a193a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b67b99c0-208c-4860-83e0-51466af787c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d43477c1ade21a66d9a75ba2d5aa042" ns2:_="">
     <xsd:import namespace="b67b99c0-208c-4860-83e0-51466af787c4"/>
@@ -1280,22 +1295,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191CB444-B9BF-4C91-94BD-600524521497}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1311,21 +1328,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20D196DE-5AC8-4D3B-8CD7-1A2AE6EEDD72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B149665-BEBB-4C97-BAA6-72374EAA67F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>